<commit_message>
Steve-1: Fix files BSA-Decomposition
</commit_message>
<xml_diff>
--- a/BSA-I/01-BSA-Decomposition/src/HC/ex01_HC_infosources.xlsx
+++ b/BSA-I/01-BSA-Decomposition/src/HC/ex01_HC_infosources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0x001\Desktop\BSA00_Decomposition-1-develop\src\HC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ALL-Projects\Solo-Leveling-21\BSA-I\01-BSA-Decomposition\src\HC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7B2D52-4FF6-4113-81D6-EF2C2747F4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4B749A-9F27-4E71-BC79-58186E5587E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A7AD035F-3D49-42E1-9766-62C4973E9B50}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>Название источника</t>
   </si>
@@ -204,12 +204,6 @@
   </si>
   <si>
     <t>Автор изменений каталога</t>
-  </si>
-  <si>
-    <t>BSA 00, 10.01.25</t>
-  </si>
-  <si>
-    <t>Sigfrydj</t>
   </si>
   <si>
     <t>Актуальность</t>
@@ -637,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31992E8-4FD0-4BBE-A664-C7369A23DBD1}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>54</v>
@@ -713,13 +707,13 @@
         <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>33</v>
@@ -742,13 +736,13 @@
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>37</v>
@@ -771,13 +765,13 @@
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>11</v>
@@ -800,13 +794,13 @@
         <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>41</v>
@@ -829,13 +823,13 @@
         <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>16</v>
@@ -858,13 +852,13 @@
         <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>45</v>
@@ -887,13 +881,13 @@
         <v>7</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>49</v>
@@ -916,13 +910,13 @@
         <v>7</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>53</v>
@@ -945,13 +939,13 @@
         <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>17</v>
@@ -974,13 +968,13 @@
         <v>21</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>22</v>
@@ -1003,13 +997,13 @@
         <v>7</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>26</v>

</xml_diff>